<commit_message>
Improve interview transcription files and translate spreadsheets to English
</commit_message>
<xml_diff>
--- a/data/Project Commits.xlsx
+++ b/data/Project Commits.xlsx
@@ -13,16 +13,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="111">
   <si>
-    <t>Título da tarefa</t>
+    <t>Task title</t>
   </si>
   <si>
-    <t>Membros do Time</t>
+    <t>Team Members</t>
   </si>
   <si>
-    <t>Descrição do commit</t>
+    <t>Commit description</t>
   </si>
   <si>
-    <t>Data</t>
+    <t>Date</t>
   </si>
   <si>
     <t>Link</t>
@@ -407,7 +407,7 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>

</xml_diff>